<commit_message>
rework finished, general text and basic decimal are ready
</commit_message>
<xml_diff>
--- a/Excelam.Tests/Files/GetCellFormat/GetCellFormatValuesDecimal.xlsx
+++ b/Excelam.Tests/Files/GetCellFormat/GetCellFormatValuesDecimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/70-yvlawy/Excelam/Dev/ExcelamSol/Excelam.Tests/Files/GetCellFormat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_F25DC773A252ABDACC1048F0A91D62385BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{122F6B37-5CE9-48AC-A1C1-D879857FE0C3}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC1048F0A91D62385BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F77D17C6-626A-4286-83F2-92EF8EC94DE8}"/>
   <bookViews>
     <workbookView xWindow="1290" yWindow="30" windowWidth="18945" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,8 +26,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="167" formatCode="0.00_ ;[Red]\-0.00\ "/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -58,11 +61,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,13 +350,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:B5"/>
+  <dimension ref="B1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
@@ -364,6 +374,26 @@
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>63.456000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>123000.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>